<commit_message>
Prima versione completa della sezione "Angolo di Brewster"
</commit_message>
<xml_diff>
--- a/Microonde/dati_brewster_rifl.xlsx
+++ b/Microonde/dati_brewster_rifl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\Stefano\Bicocca\secondo_anno\lab2\Laboratorio_2\Microonde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DACC19-4798-4F62-8DE5-2B954786EE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B0E90-0D3B-41CD-9585-7E532C56CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,6 +489,12 @@
       <c r="E5">
         <v>0.52</v>
       </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>0.08</v>
+      </c>
       <c r="I5">
         <v>35</v>
       </c>
@@ -513,10 +519,10 @@
         <v>0.12</v>
       </c>
       <c r="F6">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>0.08</v>
+        <v>0.21</v>
       </c>
       <c r="I6">
         <v>40</v>
@@ -541,6 +547,12 @@
       <c r="E7">
         <v>0.64</v>
       </c>
+      <c r="F7">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>0.11</v>
+      </c>
       <c r="I7">
         <v>50</v>
       </c>
@@ -565,10 +577,10 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="F8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G8">
-        <v>0.21</v>
+        <v>0.5</v>
       </c>
       <c r="I8">
         <v>60</v>
@@ -594,10 +606,10 @@
         <v>0.93</v>
       </c>
       <c r="F9">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G9">
-        <v>0.11</v>
+        <v>0.65</v>
       </c>
       <c r="I9">
         <v>70</v>
@@ -623,10 +635,10 @@
         <v>0.7</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>0.87</v>
       </c>
       <c r="I10">
         <v>75</v>
@@ -651,12 +663,6 @@
       <c r="E11">
         <v>0.89</v>
       </c>
-      <c r="F11">
-        <v>55</v>
-      </c>
-      <c r="G11">
-        <v>0.65</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -670,12 +676,6 @@
       </c>
       <c r="E12">
         <v>0.69</v>
-      </c>
-      <c r="F12">
-        <v>60</v>
-      </c>
-      <c r="G12">
-        <v>0.87</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>